<commit_message>
added some barrio descriptions
</commit_message>
<xml_diff>
--- a/barrio_summary.xlsx
+++ b/barrio_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/golder-mier/Documents/Georgia Tech/Spring 2019/CS6242/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{403246F0-CF3A-DF4B-86AF-FB65B8DFDBE4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4E826294-6641-1141-A850-C8409B0F86AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{9C536FFD-116C-B84F-A864-A619F1E52E38}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="barrio_summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">barrio_summary!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">barrio_summary!$A$1:$C$50</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>PALERMO</t>
   </si>
@@ -210,16 +210,7 @@
     <t xml:space="preserve">An upscale district surrounding the busiest tourist attraction – Recoleta Cemetery. The institution you have to pay attention to here is alive and kicking: la gente-bien of Recoleta, some of them pretty conservative people from families best described as “old money”. The area is busy during office hours, and quieter at night time. If you are fond of tea houses, you can find English bakery all year long. </t>
   </si>
   <si>
-    <t xml:space="preserve">You’ll see a quite neighborhood (except for when families pick up or drop off kids at school), where some good old cafes managed to survive next to new cuisines and the Starbucks of the world. You will also find young people in the area, expats and locals, partly because of “Filo” (or “Puan”), one of the University of Buenos Aires buildings. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Villa Crespo was also sometimes referred to as Palermo Queens around 2007. Palermo is considered a more expensive neighborhood and renaming Villa Crespo as part of Palermo would allow people to charge higher rents, etc. Villa Crespo has been informally associated with Buenos Aires’ Jewish community, with several synagogues located in the barrio. </t>
-  </si>
-  <si>
     <t>Almagro is between Avenidas Indepencia and Cordoba and dissected by Avenida Rivadavia – one of the city’s main thoroughfares – and has an active commercial district as well as a high population density.. Middle class.</t>
-  </si>
-  <si>
-    <t>In addition to offering a plethora of hotels, hostels and residential accommodation, the barrio has excellent transport links thus within easy reach of the city’s coveted attractions and nightlife hotspots of Palermo and San Telmo</t>
   </si>
   <si>
     <t xml:space="preserve"> Today the barrio remains a predominately industrial area, with factories providing residents with jobs. Another attraction is Club Atlético Huracán, a century-old soccer club that competes in the second tier of the Argentine soccer league and plays at the Estadio Tomás A. Ducó. The stadium itself is crumbling but has a welcoming charm, especially for true soccer enthusiasts. Tickets are often easy to come by and can usually be purchased on match days. Conveniently, the 118 bus starts and finishes its route about two blocks from the stadium, providing an easy connection to and from Palermo.</t>
@@ -262,7 +253,49 @@
     <t>It’s near Rio de la Plata with access to football clubs, tennis and recreation areas. It’s one of the oldest neighborhoods in Buenos Aires, with charming boutiques, fruit stands, restaurants and bars. Owing to its affluence, Belgrano is also popular for shopping. Avenida Cabildo runs the entire width of the barrio and is lined with a huge quantity of clothing and shoe shops ranging from chain stores to independent boutiques</t>
   </si>
   <si>
-    <t xml:space="preserve">Affluent, </t>
+    <t>Affluent, Popular</t>
+  </si>
+  <si>
+    <t>Football Team</t>
+  </si>
+  <si>
+    <t>Nuñez is a relaxed residential neighborhood popular with families with young children and professional couples. Boasting a good mix of contemporary apartment blocks, commercial streets and residential homes, Nuñez bears a similar resemblance to the northern suburbs.</t>
+  </si>
+  <si>
+    <t>Good transport system</t>
+  </si>
+  <si>
+    <t>Being predominately a residential barrio, Saavedra offers a pleasant respite from Microcentro and the popular tourist barrios. Moreover, in Parque Sarmiento it has one of the largest recreational venues in the city.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Villa Urquiza occupies a quieter zone of Buenos Aires with a blend of town houses and modern apartment blocks. If you pass by at the weekend you might just spot locals sweeping the leaves outside their homes and sharing a mate whilst chatting to their neighbors.</t>
+  </si>
+  <si>
+    <t>For those that have a desire to visit a sleepy neighborhood then Agronomía is far removed from commercialism of the ‘cooler’ Buenos Aires barrios. Resembling a spider’s web, there are three-to-four circling streets complete with crisscrossing counterparts which, for the geographically-challenged, can make getting confused a simple thing. Moreover, the circling streets and those leading off them are curiously named after major European cities; Constantinople, La Haya (The Hague) and Sofia, amongst others.</t>
+  </si>
+  <si>
+    <t>Colegiales maintains a strong residential feel that is characterized by its sleepy cobblestoned avenues lined with overhanging trees. That said, due to its close proximity to Palermo, the neighborhood is witnessing a rise in bars and restaurants</t>
+  </si>
+  <si>
+    <t>Boedo is traditionally a working class barrio situated in the mid-east area of Buenos Aires Capital Federal. The barrio is known for its influence in tango culture and its cafes were important meeting places for writers and musicians.</t>
+  </si>
+  <si>
+    <t>You’ll see a quite neighborhood (except for when families pick up or drop off kids at school), where some good old cafes managed to survive next to new cuisines and the Starbucks of the world. You will also find young people in the area, expats and locals, partly because of “Filo” (or “Puan”), one of the University of Buenos Aires buildings. For those who plan to stay a long time in Buenos Aires, the primary attraction of Caballito is that it’s a whole lot cheaper than places like Palermo, very comfortable, has some character, and yet isn’t too far from the action. It’s great value for money</t>
+  </si>
+  <si>
+    <t>Villa Crespo was also sometimes referred to as Palermo Queens around 2007. Palermo is considered a more expensive neighborhood and renaming Villa Crespo as part of Palermo would allow people to charge higher rents, etc. Villa Crespo has been informally associated with Buenos Aires’ Jewish community, with several synagogues located in the barrio. Recently Villa Crespo has started to attract a younger crowd of artistic types, who have given the barrio a distinctly cool edge.</t>
+  </si>
+  <si>
+    <t>These days, San Cristóbal is a barrio that, like parts of neighboring Balvanera, goes about its business with little fuss and is characterized by trade and industry.</t>
+  </si>
+  <si>
+    <t>In addition to offering a plethora of hotels, hostels and residential accommodation, the barrio has excellent transport links thus within easy reach of the city’s coveted attractions and nightlife hotspots of Palermo and San Telmo. Balvanera offers a fusion of working class areas (some noticeably a little rough around the edges), bohemian lifestyle and entertainment.</t>
+  </si>
+  <si>
+    <t>As it started life as a town in its own right, Flores, with its residential areas, commercial shopping district, nightlife and football club, has just about everything you can ask for and you’ll probably be able to find far cheaper rents than in the barrios further north. The A line of the Subte also stops in the barrio and provides fast access direct to Plaza de Mayo. Close to a slum.</t>
+  </si>
+  <si>
+    <t>It is the name of a middle class neighbourhood located between Belgrano, Saavedra, Núñez and Villa Urquiza; it was originally inhabited by Irish and English immigrants.</t>
   </si>
 </sst>
 </file>
@@ -624,10 +657,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C958919-B092-0A4A-AC1D-DB6931C343DC}">
-  <dimension ref="A1:D50"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +670,7 @@
     <col min="3" max="3" width="67.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -647,18 +681,24 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>12</v>
       </c>
@@ -666,10 +706,10 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -677,10 +717,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>32</v>
       </c>
@@ -688,13 +728,13 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -702,13 +742,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>24</v>
       </c>
@@ -716,18 +756,21 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>11</v>
       </c>
@@ -735,10 +778,10 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>26</v>
       </c>
@@ -746,26 +789,32 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>38</v>
       </c>
@@ -773,18 +822,21 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -792,7 +844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>21</v>
       </c>
@@ -800,7 +852,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="137" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="137" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>18</v>
       </c>
@@ -808,7 +860,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -819,7 +871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>36</v>
       </c>
@@ -830,7 +882,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>46</v>
       </c>
@@ -838,21 +890,27 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -871,7 +929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9</v>
       </c>
@@ -879,7 +937,7 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -890,7 +948,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>40</v>
       </c>
@@ -898,7 +956,7 @@
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -908,6 +966,7 @@
       <c r="B27" t="s">
         <v>27</v>
       </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -917,7 +976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>48</v>
       </c>
@@ -928,7 +987,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44</v>
       </c>
@@ -939,7 +998,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>35</v>
       </c>
@@ -950,20 +1009,26 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>15</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="19" x14ac:dyDescent="0.25">
@@ -974,7 +1039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>41</v>
       </c>
@@ -1001,7 +1066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>6</v>
       </c>
@@ -1009,7 +1074,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="19" x14ac:dyDescent="0.25">
@@ -1020,7 +1085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>23</v>
       </c>
@@ -1028,7 +1093,7 @@
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19" x14ac:dyDescent="0.25">
@@ -1095,7 +1160,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>37</v>
       </c>
@@ -1103,16 +1168,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>14</v>
       </c>
       <c r="B50" t="s">
         <v>14</v>
       </c>
+      <c r="C50" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{12DF2E8D-B5BD-7743-98CF-3F137FA79075}">
+  <autoFilter ref="A1:C50" xr:uid="{12DF2E8D-B5BD-7743-98CF-3F137FA79075}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C50">
       <sortCondition ref="B1:B50"/>
     </sortState>

</xml_diff>